<commit_message>
Fix no drift issue in default apts
</commit_message>
<xml_diff>
--- a/pwctool/data/Default AgPracticesTable ESA.xlsx
+++ b/pwctool/data/Default AgPracticesTable ESA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PWC-Prep-Tool\pwctool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63D0303-0907-4338-9F71-5D4F351FA4E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3226F3D-2FCE-4984-AB1B-6678DE03856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="37245" windowHeight="21840" tabRatio="726" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
+    <workbookView xWindow="1440" yWindow="5985" windowWidth="17700" windowHeight="13755" tabRatio="726" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
   </bookViews>
   <sheets>
     <sheet name="DefaultAPT" sheetId="25" r:id="rId1"/>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="469">
   <si>
     <t>MaxAnnNumApps</t>
   </si>
@@ -1742,9 +1742,6 @@
   <si>
     <t>Corn_gran</t>
   </si>
-  <si>
-    <t>G-NODRIFT</t>
-  </si>
 </sst>
 </file>
 
@@ -1753,7 +1750,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1853,12 +1850,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2537,8 +2528,8 @@
   </sheetPr>
   <dimension ref="A1:AH2047"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5264,7 +5255,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>469</v>
+        <v>195</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>365</v>
@@ -67556,12 +67547,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6bbb00e-98e2-4c0f-a7eb-5172b001358c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c3868428-b2d5-4b6c-aaa3-7128c526cae2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67808,20 +67801,29 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6bbb00e-98e2-4c0f-a7eb-5172b001358c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c3868428-b2d5-4b6c-aaa3-7128c526cae2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
+    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="a6bbb00e-98e2-4c0f-a7eb-5172b001358c"/>
+    <ds:schemaRef ds:uri="c3868428-b2d5-4b6c-aaa3-7128c526cae2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -67846,20 +67848,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
-    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="a6bbb00e-98e2-4c0f-a7eb-5172b001358c"/>
-    <ds:schemaRef ds:uri="c3868428-b2d5-4b6c-aaa3-7128c526cae2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add max num apps for rate 1 for corn runs in default ESA APT
</commit_message>
<xml_diff>
--- a/pwctool/data/Default AgPracticesTable ESA.xlsx
+++ b/pwctool/data/Default AgPracticesTable ESA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PWC-Prep-Tool\pwctool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3226F3D-2FCE-4984-AB1B-6678DE03856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2494B9F3-4184-42C2-B95F-335308451B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="5985" windowWidth="17700" windowHeight="13755" tabRatio="726" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
+    <workbookView xWindow="0" yWindow="945" windowWidth="35670" windowHeight="19635" tabRatio="726" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
   </bookViews>
   <sheets>
     <sheet name="DefaultAPT" sheetId="25" r:id="rId1"/>
@@ -2528,8 +2528,8 @@
   </sheetPr>
   <dimension ref="A1:AH2047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2880,7 +2880,9 @@
       <c r="N5" s="8">
         <v>0.45</v>
       </c>
-      <c r="O5" s="8"/>
+      <c r="O5" s="8">
+        <v>2</v>
+      </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8">
         <v>5</v>
@@ -2948,7 +2950,9 @@
       <c r="N6" s="8">
         <v>0.45</v>
       </c>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8">
+        <v>2</v>
+      </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="8">
         <v>5</v>
@@ -4165,7 +4169,9 @@
       <c r="N27" s="8">
         <v>0.45</v>
       </c>
-      <c r="O27" s="8"/>
+      <c r="O27" s="8">
+        <v>2</v>
+      </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8">
         <v>5</v>
@@ -4233,7 +4239,9 @@
       <c r="N28" s="8">
         <v>0.45</v>
       </c>
-      <c r="O28" s="8"/>
+      <c r="O28" s="8">
+        <v>2</v>
+      </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="8">
         <v>5</v>
@@ -67547,14 +67555,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6bbb00e-98e2-4c0f-a7eb-5172b001358c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c3868428-b2d5-4b6c-aaa3-7128c526cae2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67801,29 +67807,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6bbb00e-98e2-4c0f-a7eb-5172b001358c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c3868428-b2d5-4b6c-aaa3-7128c526cae2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
-    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="a6bbb00e-98e2-4c0f-a7eb-5172b001358c"/>
-    <ds:schemaRef ds:uri="c3868428-b2d5-4b6c-aaa3-7128c526cae2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -67848,9 +67845,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
+    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="a6bbb00e-98e2-4c0f-a7eb-5172b001358c"/>
+    <ds:schemaRef ds:uri="c3868428-b2d5-4b6c-aaa3-7128c526cae2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add max num apps for rate 1 for corn runs in default ESA APT (#17)
</commit_message>
<xml_diff>
--- a/pwctool/data/Default AgPracticesTable ESA.xlsx
+++ b/pwctool/data/Default AgPracticesTable ESA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\PWC-Prep-Tool\pwctool\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3226F3D-2FCE-4984-AB1B-6678DE03856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2494B9F3-4184-42C2-B95F-335308451B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="5985" windowWidth="17700" windowHeight="13755" tabRatio="726" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
+    <workbookView xWindow="0" yWindow="945" windowWidth="35670" windowHeight="19635" tabRatio="726" xr2:uid="{FF4C0181-D82F-49B3-A921-0560A7F629B8}"/>
   </bookViews>
   <sheets>
     <sheet name="DefaultAPT" sheetId="25" r:id="rId1"/>
@@ -2528,8 +2528,8 @@
   </sheetPr>
   <dimension ref="A1:AH2047"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2880,7 +2880,9 @@
       <c r="N5" s="8">
         <v>0.45</v>
       </c>
-      <c r="O5" s="8"/>
+      <c r="O5" s="8">
+        <v>2</v>
+      </c>
       <c r="P5" s="8"/>
       <c r="Q5" s="8">
         <v>5</v>
@@ -2948,7 +2950,9 @@
       <c r="N6" s="8">
         <v>0.45</v>
       </c>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8">
+        <v>2</v>
+      </c>
       <c r="P6" s="8"/>
       <c r="Q6" s="8">
         <v>5</v>
@@ -4165,7 +4169,9 @@
       <c r="N27" s="8">
         <v>0.45</v>
       </c>
-      <c r="O27" s="8"/>
+      <c r="O27" s="8">
+        <v>2</v>
+      </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="8">
         <v>5</v>
@@ -4233,7 +4239,9 @@
       <c r="N28" s="8">
         <v>0.45</v>
       </c>
-      <c r="O28" s="8"/>
+      <c r="O28" s="8">
+        <v>2</v>
+      </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="8">
         <v>5</v>
@@ -67547,14 +67555,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6bbb00e-98e2-4c0f-a7eb-5172b001358c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c3868428-b2d5-4b6c-aaa3-7128c526cae2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -67801,29 +67807,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a6bbb00e-98e2-4c0f-a7eb-5172b001358c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c3868428-b2d5-4b6c-aaa3-7128c526cae2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
-    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="a6bbb00e-98e2-4c0f-a7eb-5172b001358c"/>
-    <ds:schemaRef ds:uri="c3868428-b2d5-4b6c-aaa3-7128c526cae2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -67848,9 +67845,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06889177-2F4D-400B-BD60-46B96949241B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E38C3DBD-4BAB-4933-93FA-EE0DD0351B5B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bbec734e-c9c2-4352-b3fc-6a37619c639c"/>
+    <ds:schemaRef ds:uri="45003b2f-0c5d-4c18-a036-4ca6f26534cb"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="a6bbb00e-98e2-4c0f-a7eb-5172b001358c"/>
+    <ds:schemaRef ds:uri="c3868428-b2d5-4b6c-aaa3-7128c526cae2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>